<commit_message>
Fixed amt of water for 2 particle size
</commit_message>
<xml_diff>
--- a/Coordination Number & Imaging.xlsx
+++ b/Coordination Number & Imaging.xlsx
@@ -89,7 +89,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -141,7 +141,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -262,23 +262,26 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$6</c:f>
+              <c:f>Sheet1!$F$2:$F$7</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.29088820866572157</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.40724349213201022</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.52359877559829893</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.63995405906458758</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.69813170079773179</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.75630934253087612</c:v>
                 </c:pt>
               </c:numCache>
@@ -286,23 +289,26 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$6</c:f>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>2.2857099999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>4.07</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>5.3939399999999997</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>6.2777799999999999</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>6.7179500000000001</c:v>
                 </c:pt>
               </c:numCache>
@@ -347,7 +353,63 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-SG"/>
+                  <a:t>Fill Fraction</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -409,6 +471,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-SG"/>
+                  <a:t>Coordination Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1352,7 +1470,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,18 +1532,17 @@
         <v>10000</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D6" si="0">$B$15-($B$9/0.5)^3*E3</f>
-        <v>6625</v>
+        <v>7375</v>
       </c>
       <c r="E3">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F3" s="4">
-        <f t="shared" ref="F3:F6" si="1">4/3*PI()*$B$9^3*E3/$B$5^3</f>
-        <v>0.52359877559829893</v>
+        <f>4/3*PI()*$B$9^3*E3/$B$5^3</f>
+        <v>0.40724349213201022</v>
       </c>
       <c r="G3">
-        <v>4.07</v>
+        <v>2.2857099999999999</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1436,18 +1553,18 @@
         <v>1E-3</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>5875</v>
+        <f t="shared" ref="D4:D7" si="0">$B$15-($B$9/0.5)^3*E4</f>
+        <v>6625</v>
       </c>
       <c r="E4">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F4" s="4">
-        <f t="shared" si="1"/>
-        <v>0.63995405906458758</v>
+        <f t="shared" ref="F4:F7" si="1">4/3*PI()*$B$9^3*E4/$B$5^3</f>
+        <v>0.52359877559829893</v>
       </c>
       <c r="G4">
-        <v>5.3939399999999997</v>
+        <v>4.07</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1459,17 +1576,17 @@
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>5500</v>
+        <v>5875</v>
       </c>
       <c r="E5">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F5" s="4">
         <f t="shared" si="1"/>
-        <v>0.69813170079773179</v>
+        <v>0.63995405906458758</v>
       </c>
       <c r="G5">
-        <v>6.2777799999999999</v>
+        <v>5.3939399999999997</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1481,17 +1598,17 @@
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>5125</v>
+        <v>5500</v>
       </c>
       <c r="E6">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F6" s="4">
         <f t="shared" si="1"/>
-        <v>0.75630934253087612</v>
+        <v>0.69813170079773179</v>
       </c>
       <c r="G6">
-        <v>6.7179500000000001</v>
+        <v>6.2777799999999999</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1500,6 +1617,20 @@
       </c>
       <c r="B7">
         <v>4.5</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>5125</v>
+      </c>
+      <c r="E7">
+        <v>39</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" si="1"/>
+        <v>0.75630934253087612</v>
+      </c>
+      <c r="G7">
+        <v>6.7179500000000001</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>